<commit_message>
formatted a json from xsl
</commit_message>
<xml_diff>
--- a/hon_planning_and_dev.xlsx
+++ b/hon_planning_and_dev.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\desktop\projects\pivot-yarok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8314880F-118B-402E-8E12-6636CA855046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CF8EE9-FD23-4C6F-BE2E-B9AD82DF8672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="692" xr2:uid="{EE1E2518-0FD5-4401-B20A-1CAED4EDEA71}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="692" activeTab="2" xr2:uid="{EE1E2518-0FD5-4401-B20A-1CAED4EDEA71}"/>
   </bookViews>
   <sheets>
     <sheet name="מדד על תכנון" sheetId="6" r:id="rId1"/>
     <sheet name="מדד על פיתוח" sheetId="5" r:id="rId2"/>
-    <sheet name="פרופיל הון תכנון ופיתוח" sheetId="7" r:id="rId3"/>
+    <sheet name="משאב הון תכנון ופיתוח" sheetId="7" r:id="rId3"/>
     <sheet name="צללית זמנית" sheetId="8" r:id="rId4"/>
     <sheet name="נתונים שונים" sheetId="9" r:id="rId5"/>
   </sheets>
@@ -1683,12 +1683,84 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="46" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
@@ -1703,78 +1775,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="46" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1784,817 +1784,7 @@
     <cellStyle name="Normal_מקומיות 2" xfId="3" xr:uid="{02A73396-D324-4C5C-BFF3-8591E4329035}"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
-  <dxfs count="105">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -5409,8 +4599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814DFBB6-7E08-4D07-BC22-E38BA1AEF93F}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView rightToLeft="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5549,11 +4739,11 @@
         <v>10</v>
       </c>
       <c r="R2" s="38">
-        <f>N2*10/$N$14</f>
+        <f t="shared" ref="R2:R13" si="1">N2*10/$N$14</f>
         <v>4.4020546425706923</v>
       </c>
       <c r="S2" s="51">
-        <f>O2*10/$O$14</f>
+        <f t="shared" ref="S2:S13" si="2">O2*10/$O$14</f>
         <v>2.2182303991768122</v>
       </c>
       <c r="T2" s="14">
@@ -5604,7 +4794,7 @@
         <v>10</v>
       </c>
       <c r="M3" s="82">
-        <f t="shared" ref="M3:M12" si="1">C3*10</f>
+        <f t="shared" ref="M3:M12" si="3">C3*10</f>
         <v>0</v>
       </c>
       <c r="N3" s="80">
@@ -5616,23 +4806,23 @@
         <v>552.22037587690636</v>
       </c>
       <c r="P3" s="50">
-        <f t="shared" ref="P3:Q13" si="2">L3</f>
+        <f t="shared" ref="P3:Q13" si="4">L3</f>
         <v>10</v>
       </c>
       <c r="Q3" s="38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R3" s="38">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="S3" s="51">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="38">
-        <f>N3*10/$N$14</f>
         <v>10</v>
       </c>
-      <c r="S3" s="51">
-        <f>O3*10/$O$14</f>
-        <v>10</v>
-      </c>
       <c r="T3" s="14">
-        <f t="shared" ref="T3:T13" si="3">AVERAGE(P3:S3)</f>
+        <f t="shared" ref="T3:T13" si="5">AVERAGE(P3:S3)</f>
         <v>7.5</v>
       </c>
       <c r="U3" s="61" t="s">
@@ -5675,15 +4865,15 @@
         <v>17344</v>
       </c>
       <c r="L4" s="95">
-        <f t="shared" ref="L4:L13" si="4">B4</f>
+        <f t="shared" ref="L4:L13" si="6">B4</f>
         <v>10</v>
       </c>
       <c r="M4" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="N4" s="80">
-        <f t="shared" ref="N4:N13" si="5">E4*10000/H4</f>
+        <f t="shared" ref="N4:N13" si="7">E4*10000/H4</f>
         <v>5.7629312088000972</v>
       </c>
       <c r="O4" s="54">
@@ -5691,23 +4881,23 @@
         <v>178.84122527762099</v>
       </c>
       <c r="P4" s="50">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="Q4" s="38">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="R4" s="38">
+        <f t="shared" si="1"/>
+        <v>5.8991376305445948</v>
+      </c>
+      <c r="S4" s="51">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Q4" s="38">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="R4" s="38">
-        <f>N4*10/$N$14</f>
-        <v>5.8991376305445948</v>
-      </c>
-      <c r="S4" s="51">
-        <f>O4*10/$O$14</f>
         <v>3.2385843241229098</v>
       </c>
       <c r="T4" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.2844304886668763</v>
       </c>
       <c r="U4" s="61" t="s">
@@ -5749,15 +4939,15 @@
         <v>6192</v>
       </c>
       <c r="L5" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="M5" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="N5" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.3604334270826524</v>
       </c>
       <c r="O5" s="54">
@@ -5765,23 +4955,23 @@
         <v>127.11048987016898</v>
       </c>
       <c r="P5" s="50">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="Q5" s="38">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="R5" s="38">
+        <f t="shared" si="1"/>
+        <v>4.4634919250656058</v>
+      </c>
+      <c r="S5" s="51">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Q5" s="38">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="R5" s="38">
-        <f>N5*10/$N$14</f>
-        <v>4.4634919250656058</v>
-      </c>
-      <c r="S5" s="51">
-        <f>O5*10/$O$14</f>
         <v>2.3018073114075523</v>
       </c>
       <c r="T5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.6913248091182886</v>
       </c>
       <c r="U5" s="61" t="s">
@@ -5823,15 +5013,15 @@
         <v>8546</v>
       </c>
       <c r="L6" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="M6" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="N6" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.0164539690183805</v>
       </c>
       <c r="O6" s="54">
@@ -5839,23 +5029,23 @@
         <v>194.20896472878056</v>
       </c>
       <c r="P6" s="50">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="Q6" s="38">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="R6" s="38">
+        <f t="shared" si="1"/>
+        <v>5.1350174604448622</v>
+      </c>
+      <c r="S6" s="51">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Q6" s="38">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="R6" s="38">
-        <f>N6*10/$N$14</f>
-        <v>5.1350174604448622</v>
-      </c>
-      <c r="S6" s="51">
-        <f>O6*10/$O$14</f>
         <v>3.5168742989677555</v>
       </c>
       <c r="T6" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.1629729398531552</v>
       </c>
       <c r="U6" s="61" t="s">
@@ -5897,15 +5087,15 @@
         <v>2931</v>
       </c>
       <c r="L7" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="M7" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="N7" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.9026928580720699</v>
       </c>
       <c r="O7" s="54">
@@ -5913,23 +5103,23 @@
         <v>85.279542404066689</v>
       </c>
       <c r="P7" s="50">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="Q7" s="38">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="R7" s="38">
+        <f t="shared" si="1"/>
+        <v>3.9949326940350747</v>
+      </c>
+      <c r="S7" s="51">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="Q7" s="38">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="R7" s="38">
-        <f>N7*10/$N$14</f>
-        <v>3.9949326940350747</v>
-      </c>
-      <c r="S7" s="51">
-        <f>O7*10/$O$14</f>
         <v>1.5443027119136232</v>
       </c>
       <c r="T7" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.6348088514871746</v>
       </c>
       <c r="U7" s="61" t="s">
@@ -5971,14 +5161,14 @@
         <v>6774</v>
       </c>
       <c r="L8" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="M8" s="82">
         <v>5</v>
       </c>
       <c r="N8" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.8880248833592534</v>
       </c>
       <c r="O8" s="54">
@@ -5986,23 +5176,23 @@
         <v>117.67461892249072</v>
       </c>
       <c r="P8" s="50">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="Q8" s="38">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="R8" s="38">
+        <f t="shared" si="1"/>
+        <v>3.9799180429040457</v>
+      </c>
+      <c r="S8" s="51">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Q8" s="38">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="R8" s="38">
-        <f>N8*10/$N$14</f>
-        <v>3.9799180429040457</v>
-      </c>
-      <c r="S8" s="51">
-        <f>O8*10/$O$14</f>
         <v>2.1309358376287295</v>
       </c>
       <c r="T8" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.277713470133194</v>
       </c>
       <c r="U8" s="61" t="s">
@@ -6044,15 +5234,15 @@
         <v>4513</v>
       </c>
       <c r="L9" s="141">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="M9" s="142">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="N9" s="143">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.2892728509180662</v>
       </c>
       <c r="O9" s="144">
@@ -6060,23 +5250,23 @@
         <v>93.212596831661472</v>
       </c>
       <c r="P9" s="145">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="Q9" s="146">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="R9" s="146">
+        <f t="shared" si="1"/>
+        <v>5.4142843949659554</v>
+      </c>
+      <c r="S9" s="147">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="Q9" s="146">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="R9" s="146">
-        <f>N9*10/$N$14</f>
-        <v>5.4142843949659554</v>
-      </c>
-      <c r="S9" s="147">
-        <f>O9*10/$O$14</f>
         <v>1.6879601134536764</v>
       </c>
       <c r="T9" s="148">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.0255611271049077</v>
       </c>
       <c r="U9" s="61" t="s">
@@ -6118,14 +5308,14 @@
         <v>6692</v>
       </c>
       <c r="L10" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="M10" s="82">
         <v>5</v>
       </c>
       <c r="N10" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.2845743275379169</v>
       </c>
       <c r="O10" s="54">
@@ -6133,23 +5323,23 @@
         <v>124.2893970813019</v>
       </c>
       <c r="P10" s="50">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="Q10" s="38">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="R10" s="38">
+        <f t="shared" si="1"/>
+        <v>5.4094748223586144</v>
+      </c>
+      <c r="S10" s="51">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="Q10" s="38">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="R10" s="38">
-        <f>N10*10/$N$14</f>
-        <v>5.4094748223586144</v>
-      </c>
-      <c r="S10" s="51">
-        <f>O10*10/$O$14</f>
         <v>2.2507209532776611</v>
       </c>
       <c r="T10" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.9150489439090688</v>
       </c>
       <c r="U10" s="61" t="s">
@@ -6191,15 +5381,15 @@
         <v>9717</v>
       </c>
       <c r="L11" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="M11" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N11" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.7166632976214542</v>
       </c>
       <c r="O11" s="54">
@@ -6207,23 +5397,23 @@
         <v>161.64520053058968</v>
       </c>
       <c r="P11" s="50">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="Q11" s="38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="38">
+        <f t="shared" si="1"/>
+        <v>4.8281412603223801</v>
+      </c>
+      <c r="S11" s="51">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="Q11" s="38">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="38">
-        <f>N11*10/$N$14</f>
-        <v>4.8281412603223801</v>
-      </c>
-      <c r="S11" s="51">
-        <f>O11*10/$O$14</f>
         <v>2.9271864565646069</v>
       </c>
       <c r="T11" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.4388319292217466</v>
       </c>
       <c r="U11" s="61" t="s">
@@ -6265,15 +5455,15 @@
         <v>8718</v>
       </c>
       <c r="L12" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="M12" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N12" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.3267330118668994</v>
       </c>
       <c r="O12" s="54">
@@ -6281,23 +5471,23 @@
         <v>298.0193291923004</v>
       </c>
       <c r="P12" s="50">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="Q12" s="38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="38">
+        <f t="shared" si="1"/>
+        <v>6.4762648444807054</v>
+      </c>
+      <c r="S12" s="51">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="Q12" s="38">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="38">
-        <f>N12*10/$N$14</f>
-        <v>6.4762648444807054</v>
-      </c>
-      <c r="S12" s="51">
-        <f>O12*10/$O$14</f>
         <v>5.3967463391595478</v>
       </c>
       <c r="T12" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.7182527959100637</v>
       </c>
       <c r="U12" s="61" t="s">
@@ -6339,14 +5529,14 @@
         <v>3857</v>
       </c>
       <c r="L13" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="M13" s="83">
         <v>5</v>
       </c>
       <c r="N13" s="81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.7834491298067001</v>
       </c>
       <c r="O13" s="56">
@@ -6354,23 +5544,23 @@
         <v>131.4966968512816</v>
       </c>
       <c r="P13" s="52">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="Q13" s="39">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="R13" s="39">
+        <f t="shared" si="1"/>
+        <v>3.8728706497159409</v>
+      </c>
+      <c r="S13" s="53">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Q13" s="39">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="R13" s="39">
-        <f>N13*10/$N$14</f>
-        <v>3.8728706497159409</v>
-      </c>
-      <c r="S13" s="53">
-        <f>O13*10/$O$14</f>
         <v>2.3812358724081761</v>
       </c>
       <c r="T13" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.3135266305310296</v>
       </c>
       <c r="U13" s="61" t="s">
@@ -6389,51 +5579,51 @@
       <c r="G14" s="89"/>
       <c r="H14" s="101"/>
       <c r="I14" s="100">
-        <f>MAX(I2:I13)</f>
+        <f t="shared" ref="I14:T14" si="8">MAX(I2:I13)</f>
         <v>31517</v>
       </c>
       <c r="J14" s="89">
-        <f>MAX(J2:J13)</f>
+        <f t="shared" si="8"/>
         <v>34766</v>
       </c>
       <c r="K14" s="101">
-        <f>MAX(K2:K13)</f>
+        <f t="shared" si="8"/>
         <v>38736</v>
       </c>
       <c r="L14" s="102">
-        <f>MAX(L2:L13)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="M14" s="89">
-        <f>MAX(M2:M13)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="N14" s="90">
-        <f>MAX(N2:N13)</f>
+        <f t="shared" si="8"/>
         <v>9.7691079098761033</v>
       </c>
       <c r="O14" s="101">
-        <f>MAX(O2:O13)</f>
+        <f t="shared" si="8"/>
         <v>552.22037587690636</v>
       </c>
       <c r="P14" s="102">
-        <f>MAX(P2:P13)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="Q14" s="89">
-        <f>MAX(Q2:Q13)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="R14" s="89">
-        <f>MAX(R2:R13)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="S14" s="101">
-        <f>MAX(S2:S13)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="T14" s="103">
-        <f>MAX(T2:T13)</f>
+        <f t="shared" si="8"/>
         <v>7.5</v>
       </c>
       <c r="U14" s="16" t="s">
@@ -6593,149 +5783,149 @@
   <sheetData>
     <row r="1" spans="1:31" ht="22.95" customHeight="1" thickBot="1">
       <c r="A1" s="113"/>
-      <c r="B1" s="185" t="s">
+      <c r="B1" s="209" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
-      <c r="G1" s="186"/>
-      <c r="H1" s="186"/>
-      <c r="I1" s="186"/>
-      <c r="J1" s="186"/>
-      <c r="K1" s="186"/>
-      <c r="L1" s="186"/>
-      <c r="M1" s="186"/>
-      <c r="N1" s="186"/>
-      <c r="O1" s="186"/>
-      <c r="P1" s="186"/>
-      <c r="Q1" s="186"/>
-      <c r="R1" s="186"/>
-      <c r="S1" s="187"/>
-      <c r="T1" s="191" t="s">
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
+      <c r="P1" s="210"/>
+      <c r="Q1" s="210"/>
+      <c r="R1" s="210"/>
+      <c r="S1" s="211"/>
+      <c r="T1" s="193" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="192"/>
-      <c r="V1" s="192"/>
-      <c r="W1" s="192"/>
-      <c r="X1" s="193"/>
-      <c r="Y1" s="204" t="s">
+      <c r="U1" s="194"/>
+      <c r="V1" s="194"/>
+      <c r="W1" s="194"/>
+      <c r="X1" s="195"/>
+      <c r="Y1" s="181" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="205"/>
-      <c r="AA1" s="205"/>
-      <c r="AB1" s="205"/>
-      <c r="AC1" s="206"/>
+      <c r="Z1" s="182"/>
+      <c r="AA1" s="182"/>
+      <c r="AB1" s="182"/>
+      <c r="AC1" s="183"/>
       <c r="AD1" s="175" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="17.7" customHeight="1">
-      <c r="A2" s="188" t="s">
+      <c r="A2" s="190" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="208" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="181">
+      <c r="C2" s="205"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="204">
         <v>2018</v>
       </c>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="184">
+      <c r="F2" s="205"/>
+      <c r="G2" s="205"/>
+      <c r="H2" s="207"/>
+      <c r="I2" s="208">
         <v>2019</v>
       </c>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="183"/>
-      <c r="M2" s="181">
+      <c r="J2" s="205"/>
+      <c r="K2" s="205"/>
+      <c r="L2" s="207"/>
+      <c r="M2" s="204">
         <v>2020</v>
       </c>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="203"/>
-      <c r="Q2" s="184" t="s">
+      <c r="N2" s="205"/>
+      <c r="O2" s="205"/>
+      <c r="P2" s="206"/>
+      <c r="Q2" s="208" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="182"/>
-      <c r="S2" s="183"/>
-      <c r="T2" s="196" t="s">
+      <c r="R2" s="205"/>
+      <c r="S2" s="207"/>
+      <c r="T2" s="198" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="194"/>
-      <c r="V2" s="194" t="s">
+      <c r="U2" s="196"/>
+      <c r="V2" s="196" t="s">
         <v>17</v>
       </c>
-      <c r="W2" s="194"/>
+      <c r="W2" s="196"/>
       <c r="X2" s="172" t="s">
         <v>63</v>
       </c>
-      <c r="Y2" s="211" t="s">
+      <c r="Y2" s="188" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="208"/>
-      <c r="AA2" s="207" t="s">
+      <c r="Z2" s="185"/>
+      <c r="AA2" s="184" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="208"/>
+      <c r="AB2" s="185"/>
       <c r="AC2" s="173" t="s">
         <v>25</v>
       </c>
       <c r="AD2" s="176"/>
     </row>
     <row r="3" spans="1:31" s="1" customFormat="1" ht="51.75" customHeight="1">
-      <c r="A3" s="189"/>
+      <c r="A3" s="191"/>
       <c r="B3" s="170"/>
       <c r="C3" s="170"/>
       <c r="D3" s="171"/>
-      <c r="E3" s="201" t="s">
+      <c r="E3" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="199"/>
-      <c r="G3" s="199" t="s">
+      <c r="F3" s="200"/>
+      <c r="G3" s="200" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="200"/>
-      <c r="I3" s="198" t="s">
+      <c r="H3" s="201"/>
+      <c r="I3" s="199" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="199"/>
-      <c r="K3" s="199" t="s">
+      <c r="J3" s="200"/>
+      <c r="K3" s="200" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="200"/>
-      <c r="M3" s="201" t="s">
+      <c r="L3" s="201"/>
+      <c r="M3" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="199"/>
-      <c r="O3" s="199" t="s">
+      <c r="N3" s="200"/>
+      <c r="O3" s="200" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="202"/>
-      <c r="Q3" s="198" t="s">
+      <c r="P3" s="203"/>
+      <c r="Q3" s="199" t="s">
         <v>61</v>
       </c>
-      <c r="R3" s="199"/>
-      <c r="S3" s="200"/>
-      <c r="T3" s="197"/>
-      <c r="U3" s="195"/>
-      <c r="V3" s="195"/>
-      <c r="W3" s="195"/>
+      <c r="R3" s="200"/>
+      <c r="S3" s="201"/>
+      <c r="T3" s="189"/>
+      <c r="U3" s="197"/>
+      <c r="V3" s="197"/>
+      <c r="W3" s="197"/>
       <c r="X3" s="172"/>
-      <c r="Y3" s="197"/>
-      <c r="Z3" s="210"/>
-      <c r="AA3" s="209"/>
-      <c r="AB3" s="210"/>
+      <c r="Y3" s="189"/>
+      <c r="Z3" s="187"/>
+      <c r="AA3" s="186"/>
+      <c r="AB3" s="187"/>
       <c r="AC3" s="174"/>
       <c r="AD3" s="176"/>
       <c r="AE3" s="129"/>
     </row>
     <row r="4" spans="1:31" s="1" customFormat="1" ht="64.5" customHeight="1">
-      <c r="A4" s="190"/>
+      <c r="A4" s="192"/>
       <c r="B4" s="169" t="s">
         <v>13</v>
       </c>
@@ -8248,6 +7438,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="I2:L2"/>
     <mergeCell ref="Y1:AC1"/>
     <mergeCell ref="AA2:AB3"/>
     <mergeCell ref="Y2:Z3"/>
@@ -8264,10 +7458,6 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="I2:L2"/>
   </mergeCells>
   <conditionalFormatting sqref="T5:T16">
     <cfRule type="colorScale" priority="5">
@@ -8385,8 +7575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8368588A-FD19-4899-A6CF-AD984CFDAC7B}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D21"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8816,15 +8006,15 @@
         <v>53</v>
       </c>
       <c r="C4" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!B15</f>
+        <f>'משאב הון תכנון ופיתוח'!B15</f>
         <v>7.5</v>
       </c>
       <c r="D4" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!B9</f>
+        <f>'משאב הון תכנון ופיתוח'!B9</f>
         <v>5.0255611271049077</v>
       </c>
       <c r="E4" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!B17</f>
+        <f>'משאב הון תכנון ופיתוח'!B17</f>
         <v>5.4741677410091025</v>
       </c>
       <c r="F4" s="46"/>
@@ -8834,15 +8024,15 @@
         <v>54</v>
       </c>
       <c r="C5" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!C15</f>
+        <f>'משאב הון תכנון ופיתוח'!C15</f>
         <v>10</v>
       </c>
       <c r="D5" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!C9</f>
+        <f>'משאב הון תכנון ופיתוח'!C9</f>
         <v>10</v>
       </c>
       <c r="E5" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!C17</f>
+        <f>'משאב הון תכנון ופיתוח'!C17</f>
         <v>4.5769840885188779</v>
       </c>
       <c r="F5" s="46"/>
@@ -8852,15 +8042,15 @@
         <v>48</v>
       </c>
       <c r="C6" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!D15</f>
+        <f>'משאב הון תכנון ופיתוח'!D15</f>
         <v>7.5127805635524538</v>
       </c>
       <c r="D6" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!D9</f>
+        <f>'משאב הון תכנון ופיתוח'!D9</f>
         <v>7.5127805635524538</v>
       </c>
       <c r="E6" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!D17</f>
+        <f>'משאב הון תכנון ופיתוח'!D17</f>
         <v>5.5856054504256294</v>
       </c>
     </row>
@@ -8888,19 +8078,19 @@
         <v>53</v>
       </c>
       <c r="C11" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!B20</f>
+        <f>'משאב הון תכנון ופיתוח'!B20</f>
         <v>6.9834498952349353</v>
       </c>
       <c r="D11" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!B9</f>
+        <f>'משאב הון תכנון ופיתוח'!B9</f>
         <v>5.0255611271049077</v>
       </c>
       <c r="E11" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!B17</f>
+        <f>'משאב הון תכנון ופיתוח'!B17</f>
         <v>5.4741677410091025</v>
       </c>
       <c r="F11" s="48">
-        <f>'פרופיל הון תכנון ופיתוח'!B21</f>
+        <f>'משאב הון תכנון ופיתוח'!B21</f>
         <v>0.28036125375023702</v>
       </c>
       <c r="G11" s="48"/>
@@ -8910,19 +8100,19 @@
         <v>54</v>
       </c>
       <c r="C12" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!C20</f>
+        <f>'משאב הון תכנון ופיתוח'!C20</f>
         <v>7.1737080170747856</v>
       </c>
       <c r="D12" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!C9</f>
+        <f>'משאב הון תכנון ופיתוח'!C9</f>
         <v>10</v>
       </c>
       <c r="E12" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!C17</f>
+        <f>'משאב הון תכנון ופיתוח'!C17</f>
         <v>4.5769840885188779</v>
       </c>
       <c r="F12" s="48">
-        <f>'פרופיל הון תכנון ופיתוח'!C21</f>
+        <f>'משאב הון תכנון ופיתוח'!C21</f>
         <v>-0.39397923308254312</v>
       </c>
       <c r="G12" s="48"/>
@@ -8932,19 +8122,19 @@
         <v>48</v>
       </c>
       <c r="C13" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!D20</f>
+        <f>'משאב הון תכנון ופיתוח'!D20</f>
         <v>6.5163968619448758</v>
       </c>
       <c r="D13" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!D9</f>
+        <f>'משאב הון תכנון ופיתוח'!D9</f>
         <v>7.5127805635524538</v>
       </c>
       <c r="E13" s="46">
-        <f>'פרופיל הון תכנון ופיתוח'!D17</f>
+        <f>'משאב הון תכנון ופיתוח'!D17</f>
         <v>5.5856054504256294</v>
       </c>
       <c r="F13" s="48">
-        <f>'פרופיל הון תכנון ופיתוח'!D21</f>
+        <f>'משאב הון תכנון ופיתוח'!D21</f>
         <v>-0.15290408529694721</v>
       </c>
       <c r="G13" s="48"/>

</xml_diff>

<commit_message>
added a table, need needs a style
</commit_message>
<xml_diff>
--- a/hon_planning_and_dev.xlsx
+++ b/hon_planning_and_dev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\desktop\projects\pivot-yarok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22737EAD-9062-461F-B360-59907FE9CD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709C3BC8-9810-4EFE-A3EB-947D4FD46668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="692" activeTab="1" xr2:uid="{EE1E2518-0FD5-4401-B20A-1CAED4EDEA71}"/>
   </bookViews>
@@ -1754,52 +1754,91 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="53" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="55" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="54" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="55" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="53" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1820,24 +1859,24 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="46" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
@@ -1846,45 +1885,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4710,7 +4710,7 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:O1"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4726,52 +4726,52 @@
   <sheetData>
     <row r="1" spans="1:22" ht="69.599999999999994" customHeight="1" thickBot="1">
       <c r="A1" s="166"/>
-      <c r="B1" s="189" t="s">
+      <c r="B1" s="191" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="190"/>
-      <c r="K1" s="191"/>
-      <c r="L1" s="192" t="s">
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="193"/>
+      <c r="L1" s="194" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="193"/>
-      <c r="N1" s="193"/>
-      <c r="O1" s="194"/>
-      <c r="P1" s="192" t="s">
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
+      <c r="O1" s="196"/>
+      <c r="P1" s="194" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="195"/>
-      <c r="R1" s="195"/>
-      <c r="S1" s="194"/>
+      <c r="Q1" s="197"/>
+      <c r="R1" s="197"/>
+      <c r="S1" s="196"/>
       <c r="T1" s="160" t="s">
         <v>65</v>
       </c>
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="17.7" customHeight="1">
-      <c r="A2" s="222" t="s">
+      <c r="A2" s="183" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="184" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="196" t="s">
+      <c r="C2" s="185"/>
+      <c r="D2" s="184" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="197"/>
-      <c r="F2" s="196" t="s">
+      <c r="E2" s="185"/>
+      <c r="F2" s="184" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="198"/>
-      <c r="H2" s="197"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="185"/>
       <c r="I2" s="163">
         <v>2018</v>
       </c>
@@ -4784,32 +4784,32 @@
       <c r="L2" s="187" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="183" t="s">
+      <c r="M2" s="198" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="183" t="s">
+      <c r="N2" s="198" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="185" t="s">
+      <c r="O2" s="189" t="s">
         <v>29</v>
       </c>
       <c r="P2" s="187" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="183" t="s">
+      <c r="Q2" s="198" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="183" t="s">
+      <c r="R2" s="198" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="185" t="s">
+      <c r="S2" s="189" t="s">
         <v>29</v>
       </c>
       <c r="T2" s="161"/>
       <c r="V2" s="15"/>
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" ht="62.25" customHeight="1">
-      <c r="A3" s="222" t="s">
+      <c r="A3" s="183" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -4843,13 +4843,13 @@
         <v>30</v>
       </c>
       <c r="L3" s="188"/>
-      <c r="M3" s="184"/>
-      <c r="N3" s="184"/>
-      <c r="O3" s="186"/>
+      <c r="M3" s="199"/>
+      <c r="N3" s="199"/>
+      <c r="O3" s="190"/>
       <c r="P3" s="188"/>
-      <c r="Q3" s="184"/>
-      <c r="R3" s="184"/>
-      <c r="S3" s="186"/>
+      <c r="Q3" s="199"/>
+      <c r="R3" s="199"/>
+      <c r="S3" s="190"/>
       <c r="T3" s="160" t="s">
         <v>65</v>
       </c>
@@ -5835,11 +5835,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="S2:S3"/>
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="P1:S1"/>
@@ -5849,6 +5844,11 @@
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="S2:S3"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:I15">
     <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
@@ -5944,8 +5944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2FA2C2-69C4-4F73-8C4E-17B507B20ACA}">
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5962,149 +5962,149 @@
   <sheetData>
     <row r="1" spans="1:31" ht="22.95" customHeight="1" thickBot="1">
       <c r="A1" s="103"/>
-      <c r="B1" s="213" t="s">
+      <c r="B1" s="226" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="190"/>
-      <c r="K1" s="190"/>
-      <c r="L1" s="190"/>
-      <c r="M1" s="190"/>
-      <c r="N1" s="190"/>
-      <c r="O1" s="190"/>
-      <c r="P1" s="190"/>
-      <c r="Q1" s="190"/>
-      <c r="R1" s="190"/>
-      <c r="S1" s="191"/>
-      <c r="T1" s="199" t="s">
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="192"/>
+      <c r="L1" s="192"/>
+      <c r="M1" s="192"/>
+      <c r="N1" s="192"/>
+      <c r="O1" s="192"/>
+      <c r="P1" s="192"/>
+      <c r="Q1" s="192"/>
+      <c r="R1" s="192"/>
+      <c r="S1" s="193"/>
+      <c r="T1" s="212" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="200"/>
-      <c r="V1" s="200"/>
-      <c r="W1" s="200"/>
-      <c r="X1" s="201"/>
-      <c r="Y1" s="214" t="s">
+      <c r="U1" s="213"/>
+      <c r="V1" s="213"/>
+      <c r="W1" s="213"/>
+      <c r="X1" s="214"/>
+      <c r="Y1" s="200" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="215"/>
-      <c r="AA1" s="215"/>
-      <c r="AB1" s="215"/>
-      <c r="AC1" s="216"/>
+      <c r="Z1" s="201"/>
+      <c r="AA1" s="201"/>
+      <c r="AB1" s="201"/>
+      <c r="AC1" s="202"/>
       <c r="AD1" s="160" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="17.7" customHeight="1">
-      <c r="A2" s="224" t="s">
+      <c r="A2" s="209" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="184" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="198"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="211">
+      <c r="C2" s="186"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="224">
         <v>2018</v>
       </c>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="197"/>
-      <c r="I2" s="196">
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="184">
         <v>2019</v>
       </c>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="197"/>
-      <c r="M2" s="211">
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="185"/>
+      <c r="M2" s="224">
         <v>2020</v>
       </c>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
-      <c r="P2" s="212"/>
-      <c r="Q2" s="196" t="s">
+      <c r="N2" s="186"/>
+      <c r="O2" s="186"/>
+      <c r="P2" s="225"/>
+      <c r="Q2" s="184" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="198"/>
-      <c r="S2" s="197"/>
-      <c r="T2" s="204" t="s">
+      <c r="R2" s="186"/>
+      <c r="S2" s="185"/>
+      <c r="T2" s="217" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="202"/>
-      <c r="V2" s="202" t="s">
+      <c r="U2" s="215"/>
+      <c r="V2" s="215" t="s">
         <v>17</v>
       </c>
-      <c r="W2" s="202"/>
+      <c r="W2" s="215"/>
       <c r="X2" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="Y2" s="221" t="s">
+      <c r="Y2" s="207" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="218"/>
-      <c r="AA2" s="217" t="s">
+      <c r="Z2" s="204"/>
+      <c r="AA2" s="203" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="218"/>
+      <c r="AB2" s="204"/>
       <c r="AC2" s="158" t="s">
         <v>25</v>
       </c>
       <c r="AD2" s="161"/>
     </row>
     <row r="3" spans="1:31" s="1" customFormat="1" ht="51.75" customHeight="1">
-      <c r="A3" s="225"/>
+      <c r="A3" s="210"/>
       <c r="B3" s="155"/>
       <c r="C3" s="155"/>
       <c r="D3" s="156"/>
-      <c r="E3" s="209" t="s">
+      <c r="E3" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207" t="s">
+      <c r="F3" s="220"/>
+      <c r="G3" s="220" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="208"/>
-      <c r="I3" s="223" t="s">
+      <c r="H3" s="221"/>
+      <c r="I3" s="218" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="209"/>
-      <c r="K3" s="207" t="s">
+      <c r="J3" s="219"/>
+      <c r="K3" s="220" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="208"/>
-      <c r="M3" s="209" t="s">
+      <c r="L3" s="221"/>
+      <c r="M3" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="207"/>
-      <c r="O3" s="207" t="s">
+      <c r="N3" s="220"/>
+      <c r="O3" s="220" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="210"/>
-      <c r="Q3" s="206" t="s">
+      <c r="P3" s="222"/>
+      <c r="Q3" s="223" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="207"/>
-      <c r="S3" s="208"/>
-      <c r="T3" s="205"/>
-      <c r="U3" s="203"/>
-      <c r="V3" s="203"/>
-      <c r="W3" s="203"/>
+      <c r="R3" s="220"/>
+      <c r="S3" s="221"/>
+      <c r="T3" s="208"/>
+      <c r="U3" s="216"/>
+      <c r="V3" s="216"/>
+      <c r="W3" s="216"/>
       <c r="X3" s="157"/>
-      <c r="Y3" s="205"/>
-      <c r="Z3" s="220"/>
-      <c r="AA3" s="219"/>
-      <c r="AB3" s="220"/>
+      <c r="Y3" s="208"/>
+      <c r="Z3" s="206"/>
+      <c r="AA3" s="205"/>
+      <c r="AB3" s="206"/>
       <c r="AC3" s="159"/>
       <c r="AD3" s="161"/>
       <c r="AE3" s="119"/>
     </row>
     <row r="4" spans="1:31" s="1" customFormat="1" ht="64.5" customHeight="1">
-      <c r="A4" s="226"/>
+      <c r="A4" s="211"/>
       <c r="B4" s="154" t="s">
         <v>13</v>
       </c>
@@ -7589,6 +7589,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="Q2:S2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="Y1:AC1"/>
     <mergeCell ref="AA2:AB3"/>
@@ -7605,10 +7609,6 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M2:P2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="Q2:S2"/>
   </mergeCells>
   <conditionalFormatting sqref="T5:T16">
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
color in table working
</commit_message>
<xml_diff>
--- a/hon_planning_and_dev.xlsx
+++ b/hon_planning_and_dev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\desktop\projects\pivot-yarok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709C3BC8-9810-4EFE-A3EB-947D4FD46668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7158D42F-719A-4EED-A496-1C4DC8CCAADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="692" activeTab="1" xr2:uid="{EE1E2518-0FD5-4401-B20A-1CAED4EDEA71}"/>
   </bookViews>
@@ -294,7 +294,7 @@
     <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1757,6 +1757,45 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="54" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="55" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="53" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
@@ -1766,44 +1805,11 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="53" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="55" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="54" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1877,14 +1883,8 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4713,7 +4713,7 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
@@ -4724,54 +4724,54 @@
     <col min="21" max="21" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="69.599999999999994" customHeight="1" thickBot="1">
+    <row r="1" spans="1:22" ht="69.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="166"/>
-      <c r="B1" s="191" t="s">
+      <c r="B1" s="184" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
-      <c r="E1" s="192"/>
-      <c r="F1" s="192"/>
-      <c r="G1" s="192"/>
-      <c r="H1" s="192"/>
-      <c r="I1" s="192"/>
-      <c r="J1" s="192"/>
-      <c r="K1" s="193"/>
-      <c r="L1" s="194" t="s">
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="185"/>
+      <c r="K1" s="186"/>
+      <c r="L1" s="187" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="195"/>
-      <c r="N1" s="195"/>
-      <c r="O1" s="196"/>
-      <c r="P1" s="194" t="s">
+      <c r="M1" s="188"/>
+      <c r="N1" s="188"/>
+      <c r="O1" s="189"/>
+      <c r="P1" s="187" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="197"/>
-      <c r="R1" s="197"/>
-      <c r="S1" s="196"/>
+      <c r="Q1" s="190"/>
+      <c r="R1" s="190"/>
+      <c r="S1" s="189"/>
       <c r="T1" s="160" t="s">
         <v>65</v>
       </c>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" ht="17.7" customHeight="1">
+    <row r="2" spans="1:22" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="183" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="197" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="185"/>
-      <c r="D2" s="184" t="s">
+      <c r="C2" s="198"/>
+      <c r="D2" s="197" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="185"/>
-      <c r="F2" s="184" t="s">
+      <c r="E2" s="198"/>
+      <c r="F2" s="197" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="186"/>
-      <c r="H2" s="185"/>
+      <c r="G2" s="199"/>
+      <c r="H2" s="198"/>
       <c r="I2" s="163">
         <v>2018</v>
       </c>
@@ -4781,34 +4781,34 @@
       <c r="K2" s="165">
         <v>2020</v>
       </c>
-      <c r="L2" s="187" t="s">
+      <c r="L2" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="198" t="s">
+      <c r="M2" s="191" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="198" t="s">
+      <c r="N2" s="191" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="189" t="s">
+      <c r="O2" s="193" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="187" t="s">
+      <c r="P2" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="198" t="s">
+      <c r="Q2" s="191" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="198" t="s">
+      <c r="R2" s="191" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="189" t="s">
+      <c r="S2" s="193" t="s">
         <v>29</v>
       </c>
       <c r="T2" s="161"/>
       <c r="V2" s="15"/>
     </row>
-    <row r="3" spans="1:22" s="1" customFormat="1" ht="62.25" customHeight="1">
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="183" t="s">
         <v>64</v>
       </c>
@@ -4842,21 +4842,21 @@
       <c r="K3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="188"/>
-      <c r="M3" s="199"/>
-      <c r="N3" s="199"/>
-      <c r="O3" s="190"/>
-      <c r="P3" s="188"/>
-      <c r="Q3" s="199"/>
-      <c r="R3" s="199"/>
-      <c r="S3" s="190"/>
+      <c r="L3" s="196"/>
+      <c r="M3" s="192"/>
+      <c r="N3" s="192"/>
+      <c r="O3" s="194"/>
+      <c r="P3" s="196"/>
+      <c r="Q3" s="192"/>
+      <c r="R3" s="192"/>
+      <c r="S3" s="194"/>
       <c r="T3" s="160" t="s">
         <v>65</v>
       </c>
       <c r="U3" s="167"/>
       <c r="V3" s="15"/>
     </row>
-    <row r="4" spans="1:22" s="15" customFormat="1" ht="13.5" customHeight="1">
+    <row r="4" spans="1:22" s="15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="84" t="s">
         <v>0</v>
       </c>
@@ -4928,7 +4928,7 @@
       </c>
       <c r="U4" s="53"/>
     </row>
-    <row r="5" spans="1:22" s="15" customFormat="1">
+    <row r="5" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="84" t="s">
         <v>1</v>
       </c>
@@ -5000,7 +5000,7 @@
       </c>
       <c r="U5" s="53"/>
     </row>
-    <row r="6" spans="1:22" s="15" customFormat="1">
+    <row r="6" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="84" t="s">
         <v>2</v>
       </c>
@@ -5072,7 +5072,7 @@
       </c>
       <c r="U6" s="53"/>
     </row>
-    <row r="7" spans="1:22" s="15" customFormat="1">
+    <row r="7" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="84" t="s">
         <v>3</v>
       </c>
@@ -5144,7 +5144,7 @@
       </c>
       <c r="U7" s="53"/>
     </row>
-    <row r="8" spans="1:22" s="15" customFormat="1">
+    <row r="8" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="84" t="s">
         <v>4</v>
       </c>
@@ -5216,7 +5216,7 @@
       </c>
       <c r="U8" s="53"/>
     </row>
-    <row r="9" spans="1:22" s="15" customFormat="1">
+    <row r="9" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="84" t="s">
         <v>5</v>
       </c>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="U9" s="53"/>
     </row>
-    <row r="10" spans="1:22" s="15" customFormat="1">
+    <row r="10" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="84" t="s">
         <v>6</v>
       </c>
@@ -5359,7 +5359,7 @@
       </c>
       <c r="U10" s="53"/>
     </row>
-    <row r="11" spans="1:22" s="15" customFormat="1">
+    <row r="11" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="122" t="s">
         <v>7</v>
       </c>
@@ -5431,7 +5431,7 @@
       </c>
       <c r="U11" s="53"/>
     </row>
-    <row r="12" spans="1:22" s="15" customFormat="1">
+    <row r="12" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="84" t="s">
         <v>8</v>
       </c>
@@ -5502,7 +5502,7 @@
       </c>
       <c r="U12" s="53"/>
     </row>
-    <row r="13" spans="1:22" s="15" customFormat="1">
+    <row r="13" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="84" t="s">
         <v>9</v>
       </c>
@@ -5574,7 +5574,7 @@
       </c>
       <c r="U13" s="53"/>
     </row>
-    <row r="14" spans="1:22" s="15" customFormat="1">
+    <row r="14" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="84" t="s">
         <v>10</v>
       </c>
@@ -5646,7 +5646,7 @@
       </c>
       <c r="U14" s="53"/>
     </row>
-    <row r="15" spans="1:22" s="15" customFormat="1" ht="15" thickBot="1">
+    <row r="15" spans="1:22" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="85" t="s">
         <v>11</v>
       </c>
@@ -5717,7 +5717,7 @@
       </c>
       <c r="U15" s="53"/>
     </row>
-    <row r="16" spans="1:22" s="15" customFormat="1" thickBot="1">
+    <row r="16" spans="1:22" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="83"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
@@ -5735,7 +5735,7 @@
       <c r="S16" s="17"/>
       <c r="T16" s="17"/>
     </row>
-    <row r="17" spans="1:21" s="15" customFormat="1" thickBot="1">
+    <row r="17" spans="1:21" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="91" t="s">
         <v>12</v>
       </c>
@@ -5796,39 +5796,39 @@
       </c>
       <c r="U17" s="16"/>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="102"/>
       <c r="B20" s="78"/>
       <c r="C20" s="79"/>
       <c r="D20" s="78"/>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B26" s="78"/>
       <c r="C26" s="79"/>
       <c r="D26" s="78"/>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="102"/>
       <c r="B27" s="78"/>
       <c r="C27" s="79"/>
       <c r="D27" s="78"/>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B28" s="78"/>
       <c r="C28" s="101"/>
       <c r="D28" s="78"/>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B29" s="78"/>
       <c r="C29" s="35"/>
       <c r="D29" s="78"/>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B30" s="78"/>
       <c r="C30" s="101"/>
       <c r="D30" s="78"/>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B31" s="78"/>
       <c r="C31" s="79"/>
       <c r="D31" s="78"/>
@@ -5944,11 +5944,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2FA2C2-69C4-4F73-8C4E-17B507B20ACA}">
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="19" width="9.44140625" customWidth="1"/>
@@ -5960,151 +5960,151 @@
     <col min="31" max="31" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="22.95" customHeight="1" thickBot="1">
+    <row r="1" spans="1:31" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="103"/>
-      <c r="B1" s="226" t="s">
+      <c r="B1" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
-      <c r="E1" s="192"/>
-      <c r="F1" s="192"/>
-      <c r="G1" s="192"/>
-      <c r="H1" s="192"/>
-      <c r="I1" s="192"/>
-      <c r="J1" s="192"/>
-      <c r="K1" s="192"/>
-      <c r="L1" s="192"/>
-      <c r="M1" s="192"/>
-      <c r="N1" s="192"/>
-      <c r="O1" s="192"/>
-      <c r="P1" s="192"/>
-      <c r="Q1" s="192"/>
-      <c r="R1" s="192"/>
-      <c r="S1" s="193"/>
-      <c r="T1" s="212" t="s">
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="185"/>
+      <c r="K1" s="185"/>
+      <c r="L1" s="185"/>
+      <c r="M1" s="185"/>
+      <c r="N1" s="185"/>
+      <c r="O1" s="185"/>
+      <c r="P1" s="185"/>
+      <c r="Q1" s="185"/>
+      <c r="R1" s="185"/>
+      <c r="S1" s="186"/>
+      <c r="T1" s="214" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="213"/>
-      <c r="V1" s="213"/>
-      <c r="W1" s="213"/>
-      <c r="X1" s="214"/>
-      <c r="Y1" s="200" t="s">
+      <c r="U1" s="215"/>
+      <c r="V1" s="215"/>
+      <c r="W1" s="215"/>
+      <c r="X1" s="216"/>
+      <c r="Y1" s="202" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="201"/>
-      <c r="AA1" s="201"/>
-      <c r="AB1" s="201"/>
-      <c r="AC1" s="202"/>
+      <c r="Z1" s="203"/>
+      <c r="AA1" s="203"/>
+      <c r="AB1" s="203"/>
+      <c r="AC1" s="204"/>
       <c r="AD1" s="160" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="17.7" customHeight="1">
-      <c r="A2" s="209" t="s">
+    <row r="2" spans="1:31" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="211" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="197" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="186"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="224">
+      <c r="C2" s="199"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="200">
         <v>2018</v>
       </c>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="185"/>
-      <c r="I2" s="184">
+      <c r="F2" s="199"/>
+      <c r="G2" s="199"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="197">
         <v>2019</v>
       </c>
-      <c r="J2" s="186"/>
-      <c r="K2" s="186"/>
-      <c r="L2" s="185"/>
-      <c r="M2" s="224">
+      <c r="J2" s="199"/>
+      <c r="K2" s="199"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="200">
         <v>2020</v>
       </c>
-      <c r="N2" s="186"/>
-      <c r="O2" s="186"/>
-      <c r="P2" s="225"/>
-      <c r="Q2" s="184" t="s">
+      <c r="N2" s="199"/>
+      <c r="O2" s="199"/>
+      <c r="P2" s="226"/>
+      <c r="Q2" s="197" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="186"/>
-      <c r="S2" s="185"/>
-      <c r="T2" s="217" t="s">
+      <c r="R2" s="199"/>
+      <c r="S2" s="198"/>
+      <c r="T2" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="215"/>
-      <c r="V2" s="215" t="s">
+      <c r="U2" s="217"/>
+      <c r="V2" s="217" t="s">
         <v>17</v>
       </c>
-      <c r="W2" s="215"/>
+      <c r="W2" s="217"/>
       <c r="X2" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="Y2" s="207" t="s">
+      <c r="Y2" s="209" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="204"/>
-      <c r="AA2" s="203" t="s">
+      <c r="Z2" s="206"/>
+      <c r="AA2" s="205" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="204"/>
+      <c r="AB2" s="206"/>
       <c r="AC2" s="158" t="s">
         <v>25</v>
       </c>
       <c r="AD2" s="161"/>
     </row>
-    <row r="3" spans="1:31" s="1" customFormat="1" ht="51.75" customHeight="1">
-      <c r="A3" s="210"/>
+    <row r="3" spans="1:31" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="212"/>
       <c r="B3" s="155"/>
       <c r="C3" s="155"/>
       <c r="D3" s="156"/>
-      <c r="E3" s="219" t="s">
+      <c r="E3" s="221" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="220"/>
-      <c r="G3" s="220" t="s">
+      <c r="F3" s="222"/>
+      <c r="G3" s="222" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="221"/>
-      <c r="I3" s="218" t="s">
+      <c r="H3" s="223"/>
+      <c r="I3" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="219"/>
-      <c r="K3" s="220" t="s">
+      <c r="J3" s="221"/>
+      <c r="K3" s="222" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="221"/>
-      <c r="M3" s="219" t="s">
+      <c r="L3" s="223"/>
+      <c r="M3" s="221" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="220"/>
-      <c r="O3" s="220" t="s">
+      <c r="N3" s="222"/>
+      <c r="O3" s="222" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="222"/>
-      <c r="Q3" s="223" t="s">
+      <c r="P3" s="224"/>
+      <c r="Q3" s="225" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="220"/>
-      <c r="S3" s="221"/>
-      <c r="T3" s="208"/>
-      <c r="U3" s="216"/>
-      <c r="V3" s="216"/>
-      <c r="W3" s="216"/>
+      <c r="R3" s="222"/>
+      <c r="S3" s="223"/>
+      <c r="T3" s="210"/>
+      <c r="U3" s="218"/>
+      <c r="V3" s="218"/>
+      <c r="W3" s="218"/>
       <c r="X3" s="157"/>
-      <c r="Y3" s="208"/>
-      <c r="Z3" s="206"/>
-      <c r="AA3" s="205"/>
-      <c r="AB3" s="206"/>
+      <c r="Y3" s="210"/>
+      <c r="Z3" s="208"/>
+      <c r="AA3" s="207"/>
+      <c r="AB3" s="208"/>
       <c r="AC3" s="159"/>
       <c r="AD3" s="161"/>
       <c r="AE3" s="119"/>
     </row>
-    <row r="4" spans="1:31" s="1" customFormat="1" ht="64.5" customHeight="1">
-      <c r="A4" s="211"/>
+    <row r="4" spans="1:31" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="213"/>
       <c r="B4" s="154" t="s">
         <v>13</v>
       </c>
@@ -6194,7 +6194,7 @@
       </c>
       <c r="AE4" s="162"/>
     </row>
-    <row r="5" spans="1:31" s="15" customFormat="1" ht="13.5" customHeight="1">
+    <row r="5" spans="1:31" s="15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="84" t="s">
         <v>0</v>
       </c>
@@ -6298,7 +6298,7 @@
       </c>
       <c r="AE5" s="53"/>
     </row>
-    <row r="6" spans="1:31" s="15" customFormat="1" ht="13.8">
+    <row r="6" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="84" t="s">
         <v>1</v>
       </c>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="AE6" s="53"/>
     </row>
-    <row r="7" spans="1:31" s="15" customFormat="1" ht="13.8">
+    <row r="7" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="84" t="s">
         <v>2</v>
       </c>
@@ -6506,7 +6506,7 @@
       </c>
       <c r="AE7" s="53"/>
     </row>
-    <row r="8" spans="1:31" s="15" customFormat="1" ht="13.8">
+    <row r="8" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="84" t="s">
         <v>3</v>
       </c>
@@ -6610,7 +6610,7 @@
       </c>
       <c r="AE8" s="53"/>
     </row>
-    <row r="9" spans="1:31" s="15" customFormat="1" ht="13.8">
+    <row r="9" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="84" t="s">
         <v>4</v>
       </c>
@@ -6714,7 +6714,7 @@
       </c>
       <c r="AE9" s="53"/>
     </row>
-    <row r="10" spans="1:31" s="15" customFormat="1" ht="13.8">
+    <row r="10" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="84" t="s">
         <v>5</v>
       </c>
@@ -6818,7 +6818,7 @@
       </c>
       <c r="AE10" s="53"/>
     </row>
-    <row r="11" spans="1:31" s="15" customFormat="1" ht="13.8">
+    <row r="11" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="84" t="s">
         <v>6</v>
       </c>
@@ -6922,7 +6922,7 @@
       </c>
       <c r="AE11" s="53"/>
     </row>
-    <row r="12" spans="1:31" s="121" customFormat="1" ht="13.8">
+    <row r="12" spans="1:31" s="121" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="122" t="s">
         <v>7</v>
       </c>
@@ -7026,7 +7026,7 @@
       </c>
       <c r="AE12" s="120"/>
     </row>
-    <row r="13" spans="1:31" s="15" customFormat="1" ht="13.8">
+    <row r="13" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="84" t="s">
         <v>8</v>
       </c>
@@ -7130,7 +7130,7 @@
       </c>
       <c r="AE13" s="53"/>
     </row>
-    <row r="14" spans="1:31" s="15" customFormat="1" ht="13.8">
+    <row r="14" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="84" t="s">
         <v>9</v>
       </c>
@@ -7234,7 +7234,7 @@
       </c>
       <c r="AE14" s="53"/>
     </row>
-    <row r="15" spans="1:31" s="15" customFormat="1" ht="13.8">
+    <row r="15" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="84" t="s">
         <v>10</v>
       </c>
@@ -7338,7 +7338,7 @@
       </c>
       <c r="AE15" s="53"/>
     </row>
-    <row r="16" spans="1:31" s="15" customFormat="1" thickBot="1">
+    <row r="16" spans="1:31" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="85" t="s">
         <v>11</v>
       </c>
@@ -7442,7 +7442,7 @@
       </c>
       <c r="AE16" s="53"/>
     </row>
-    <row r="17" spans="1:31" s="15" customFormat="1" thickBot="1">
+    <row r="17" spans="1:31" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="83"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -7474,7 +7474,7 @@
       <c r="AC17" s="17"/>
       <c r="AD17" s="17"/>
     </row>
-    <row r="18" spans="1:31" s="15" customFormat="1" thickBot="1">
+    <row r="18" spans="1:31" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="91" t="s">
         <v>12</v>
       </c>
@@ -7589,11 +7589,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="I2:L2"/>
     <mergeCell ref="Y1:AC1"/>
     <mergeCell ref="AA2:AB3"/>
     <mergeCell ref="Y2:Z3"/>
@@ -7609,6 +7604,11 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M2:P2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="I2:L2"/>
   </mergeCells>
   <conditionalFormatting sqref="T5:T16">
     <cfRule type="colorScale" priority="5">
@@ -7730,14 +7730,14 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" style="39" customWidth="1"/>
     <col min="2" max="3" width="14.109375" style="39" customWidth="1"/>
     <col min="4" max="5" width="12.88671875" style="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>39</v>
       </c>
@@ -7752,7 +7752,7 @@
       </c>
       <c r="E1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
@@ -7770,7 +7770,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>1</v>
       </c>
@@ -7788,7 +7788,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>2</v>
       </c>
@@ -7806,7 +7806,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
         <v>3</v>
       </c>
@@ -7824,7 +7824,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
@@ -7842,7 +7842,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
         <v>5</v>
       </c>
@@ -7860,7 +7860,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>6</v>
       </c>
@@ -7878,7 +7878,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
         <v>7</v>
       </c>
@@ -7896,7 +7896,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
         <v>8</v>
       </c>
@@ -7914,7 +7914,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
         <v>9</v>
       </c>
@@ -7932,7 +7932,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="34" t="s">
         <v>10</v>
       </c>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="34" t="s">
         <v>11</v>
       </c>
@@ -7968,13 +7968,13 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="39" t="s">
         <v>41</v>
       </c>
@@ -7992,7 +7992,7 @@
       </c>
       <c r="E15" s="40"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="39" t="s">
         <v>42</v>
       </c>
@@ -8011,7 +8011,7 @@
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="39" t="s">
         <v>40</v>
       </c>
@@ -8030,7 +8030,7 @@
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="39" t="s">
         <v>43</v>
       </c>
@@ -8049,7 +8049,7 @@
       <c r="E19" s="40"/>
       <c r="F19" s="40"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="39" t="s">
         <v>44</v>
       </c>
@@ -8068,7 +8068,7 @@
       <c r="E20" s="40"/>
       <c r="F20" s="40"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="39" t="s">
         <v>45</v>
       </c>
@@ -8087,7 +8087,7 @@
       <c r="E21" s="41"/>
       <c r="F21" s="41"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="41">
         <f>B9/B20</f>
         <v>0.71963874624976298</v>
@@ -8134,13 +8134,13 @@
       <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="30" customHeight="1"/>
-    <row r="3" spans="2:7">
+    <row r="1" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>46</v>
       </c>
@@ -8152,7 +8152,7 @@
       </c>
       <c r="F3" s="42"/>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>52</v>
       </c>
@@ -8170,7 +8170,7 @@
       </c>
       <c r="F4" s="42"/>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>53</v>
       </c>
@@ -8188,7 +8188,7 @@
       </c>
       <c r="F5" s="42"/>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="43" t="s">
         <v>47</v>
       </c>
@@ -8205,12 +8205,12 @@
         <v>5.5856054504256294</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>44</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>52</v>
       </c>
@@ -8246,7 +8246,7 @@
       </c>
       <c r="G11" s="44"/>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>53</v>
       </c>
@@ -8268,7 +8268,7 @@
       </c>
       <c r="G12" s="44"/>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="43" t="s">
         <v>47</v>
       </c>
@@ -8290,16 +8290,16 @@
       </c>
       <c r="G13" s="44"/>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C14" s="42"/>
       <c r="D14" s="42"/>
       <c r="E14" s="42"/>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D15" s="42"/>
       <c r="E15" s="42"/>
     </row>
-    <row r="16" spans="2:7">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
@@ -8307,11 +8307,11 @@
       <c r="F16" s="44"/>
       <c r="G16" s="44"/>
     </row>
-    <row r="17" spans="4:5">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
     </row>
-    <row r="18" spans="4:5">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D18" s="45"/>
       <c r="E18" s="42"/>
     </row>
@@ -8329,25 +8329,25 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="35"/>
       <c r="B1" s="50" t="s">
         <v>51</v>
       </c>
       <c r="C1" s="35"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="49" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>0</v>
       </c>
@@ -8358,7 +8358,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
         <v>1</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
         <v>2</v>
       </c>
@@ -8380,7 +8380,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
         <v>3</v>
       </c>
@@ -8391,7 +8391,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>4</v>
       </c>
@@ -8402,7 +8402,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
         <v>5</v>
       </c>
@@ -8413,7 +8413,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
         <v>6</v>
       </c>
@@ -8424,7 +8424,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
         <v>7</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="34" t="s">
         <v>8</v>
       </c>
@@ -8446,7 +8446,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="34" t="s">
         <v>9</v>
       </c>
@@ -8457,7 +8457,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="34" t="s">
         <v>10</v>
       </c>
@@ -8468,7 +8468,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
reading measurement dyanmically based on name of the sheet, and table style complete
</commit_message>
<xml_diff>
--- a/hon_planning_and_dev.xlsx
+++ b/hon_planning_and_dev.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\desktop\projects\pivot-yarok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7158D42F-719A-4EED-A496-1C4DC8CCAADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA69EED3-11AD-45DF-B945-EAB9433BDB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="692" activeTab="1" xr2:uid="{EE1E2518-0FD5-4401-B20A-1CAED4EDEA71}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="692" xr2:uid="{EE1E2518-0FD5-4401-B20A-1CAED4EDEA71}"/>
   </bookViews>
   <sheets>
     <sheet name="מדד על תכנון" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="73">
   <si>
     <t>אופקים</t>
   </si>
@@ -294,7 +294,7 @@
     <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,7 +509,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="56">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1185,45 +1185,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1232,7 +1193,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1778,24 +1739,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="54" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="55" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="53" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
@@ -1805,86 +1748,95 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="46" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="46" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4709,11 +4661,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814DFBB6-7E08-4D07-BC22-E38BA1AEF93F}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
@@ -4724,7 +4676,7 @@
     <col min="21" max="21" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="69.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="69.599999999999994" customHeight="1" thickBot="1">
       <c r="A1" s="166"/>
       <c r="B1" s="184" t="s">
         <v>68</v>
@@ -4755,23 +4707,23 @@
       </c>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="17.7" customHeight="1">
       <c r="A2" s="183" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="197" t="s">
+      <c r="B2" s="191" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="198"/>
-      <c r="D2" s="197" t="s">
+      <c r="C2" s="192"/>
+      <c r="D2" s="191" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="198"/>
-      <c r="F2" s="197" t="s">
+      <c r="E2" s="192"/>
+      <c r="F2" s="191" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="199"/>
-      <c r="H2" s="198"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="192"/>
       <c r="I2" s="163">
         <v>2018</v>
       </c>
@@ -4781,37 +4733,35 @@
       <c r="K2" s="165">
         <v>2020</v>
       </c>
-      <c r="L2" s="195" t="s">
+      <c r="L2" s="219" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="191" t="s">
+      <c r="M2" s="218" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="191" t="s">
+      <c r="N2" s="218" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="193" t="s">
+      <c r="O2" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="195" t="s">
+      <c r="P2" s="219" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="191" t="s">
+      <c r="Q2" s="218" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="191" t="s">
+      <c r="R2" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="193" t="s">
+      <c r="S2" s="158" t="s">
         <v>29</v>
       </c>
       <c r="T2" s="161"/>
       <c r="V2" s="15"/>
     </row>
-    <row r="3" spans="1:22" s="1" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="183" t="s">
-        <v>64</v>
-      </c>
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="62.25" customHeight="1">
+      <c r="A3" s="223"/>
       <c r="B3" s="5" t="s">
         <v>32</v>
       </c>
@@ -4842,21 +4792,37 @@
       <c r="K3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="196"/>
-      <c r="M3" s="192"/>
-      <c r="N3" s="192"/>
-      <c r="O3" s="194"/>
-      <c r="P3" s="196"/>
-      <c r="Q3" s="192"/>
-      <c r="R3" s="192"/>
-      <c r="S3" s="194"/>
+      <c r="L3" s="219" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="218" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="218" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="219" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="218" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="218" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="158" t="s">
+        <v>29</v>
+      </c>
       <c r="T3" s="160" t="s">
         <v>65</v>
       </c>
       <c r="U3" s="167"/>
       <c r="V3" s="15"/>
     </row>
-    <row r="4" spans="1:22" s="15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="15" customFormat="1" ht="13.5" customHeight="1">
       <c r="A4" s="84" t="s">
         <v>0</v>
       </c>
@@ -4928,7 +4894,7 @@
       </c>
       <c r="U4" s="53"/>
     </row>
-    <row r="5" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="15" customFormat="1">
       <c r="A5" s="84" t="s">
         <v>1</v>
       </c>
@@ -5000,7 +4966,7 @@
       </c>
       <c r="U5" s="53"/>
     </row>
-    <row r="6" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="15" customFormat="1">
       <c r="A6" s="84" t="s">
         <v>2</v>
       </c>
@@ -5072,7 +5038,7 @@
       </c>
       <c r="U6" s="53"/>
     </row>
-    <row r="7" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="15" customFormat="1">
       <c r="A7" s="84" t="s">
         <v>3</v>
       </c>
@@ -5144,7 +5110,7 @@
       </c>
       <c r="U7" s="53"/>
     </row>
-    <row r="8" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="15" customFormat="1">
       <c r="A8" s="84" t="s">
         <v>4</v>
       </c>
@@ -5216,7 +5182,7 @@
       </c>
       <c r="U8" s="53"/>
     </row>
-    <row r="9" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="15" customFormat="1">
       <c r="A9" s="84" t="s">
         <v>5</v>
       </c>
@@ -5288,7 +5254,7 @@
       </c>
       <c r="U9" s="53"/>
     </row>
-    <row r="10" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="15" customFormat="1">
       <c r="A10" s="84" t="s">
         <v>6</v>
       </c>
@@ -5359,7 +5325,7 @@
       </c>
       <c r="U10" s="53"/>
     </row>
-    <row r="11" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="15" customFormat="1">
       <c r="A11" s="122" t="s">
         <v>7</v>
       </c>
@@ -5431,7 +5397,7 @@
       </c>
       <c r="U11" s="53"/>
     </row>
-    <row r="12" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="15" customFormat="1">
       <c r="A12" s="84" t="s">
         <v>8</v>
       </c>
@@ -5502,7 +5468,7 @@
       </c>
       <c r="U12" s="53"/>
     </row>
-    <row r="13" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="15" customFormat="1">
       <c r="A13" s="84" t="s">
         <v>9</v>
       </c>
@@ -5574,7 +5540,7 @@
       </c>
       <c r="U13" s="53"/>
     </row>
-    <row r="14" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="15" customFormat="1">
       <c r="A14" s="84" t="s">
         <v>10</v>
       </c>
@@ -5646,7 +5612,7 @@
       </c>
       <c r="U14" s="53"/>
     </row>
-    <row r="15" spans="1:22" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" s="15" customFormat="1" ht="15" thickBot="1">
       <c r="A15" s="85" t="s">
         <v>11</v>
       </c>
@@ -5717,7 +5683,7 @@
       </c>
       <c r="U15" s="53"/>
     </row>
-    <row r="16" spans="1:22" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="15" customFormat="1" thickBot="1">
       <c r="A16" s="83"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
@@ -5735,7 +5701,7 @@
       <c r="S16" s="17"/>
       <c r="T16" s="17"/>
     </row>
-    <row r="17" spans="1:21" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" s="15" customFormat="1" thickBot="1">
       <c r="A17" s="91" t="s">
         <v>12</v>
       </c>
@@ -5796,59 +5762,51 @@
       </c>
       <c r="U17" s="16"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21">
       <c r="A20" s="102"/>
       <c r="B20" s="78"/>
       <c r="C20" s="79"/>
       <c r="D20" s="78"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21">
       <c r="B26" s="78"/>
       <c r="C26" s="79"/>
       <c r="D26" s="78"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21">
       <c r="A27" s="102"/>
       <c r="B27" s="78"/>
       <c r="C27" s="79"/>
       <c r="D27" s="78"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21">
       <c r="B28" s="78"/>
       <c r="C28" s="101"/>
       <c r="D28" s="78"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21">
       <c r="B29" s="78"/>
       <c r="C29" s="35"/>
       <c r="D29" s="78"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21">
       <c r="B30" s="78"/>
       <c r="C30" s="101"/>
       <c r="D30" s="78"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21">
       <c r="B31" s="78"/>
       <c r="C31" s="79"/>
       <c r="D31" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="6">
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="P1:S1"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:H2"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="S2:S3"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:I15">
     <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
@@ -5944,11 +5902,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2FA2C2-69C4-4F73-8C4E-17B507B20ACA}">
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView rightToLeft="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="19" width="9.44140625" customWidth="1"/>
@@ -5960,9 +5918,9 @@
     <col min="31" max="31" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" ht="22.95" customHeight="1" thickBot="1">
       <c r="A1" s="103"/>
-      <c r="B1" s="201" t="s">
+      <c r="B1" s="217" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="185"/>
@@ -5982,129 +5940,129 @@
       <c r="Q1" s="185"/>
       <c r="R1" s="185"/>
       <c r="S1" s="186"/>
-      <c r="T1" s="214" t="s">
+      <c r="T1" s="203" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="215"/>
-      <c r="V1" s="215"/>
-      <c r="W1" s="215"/>
-      <c r="X1" s="216"/>
-      <c r="Y1" s="202" t="s">
+      <c r="U1" s="204"/>
+      <c r="V1" s="204"/>
+      <c r="W1" s="204"/>
+      <c r="X1" s="205"/>
+      <c r="Y1" s="194" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="203"/>
-      <c r="AA1" s="203"/>
-      <c r="AB1" s="203"/>
-      <c r="AC1" s="204"/>
+      <c r="Z1" s="195"/>
+      <c r="AA1" s="195"/>
+      <c r="AB1" s="195"/>
+      <c r="AC1" s="196"/>
       <c r="AD1" s="160" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="211" t="s">
+    <row r="2" spans="1:31" ht="17.7" customHeight="1">
+      <c r="A2" s="220" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="197" t="s">
+      <c r="B2" s="191" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="199"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="200">
+      <c r="C2" s="193"/>
+      <c r="D2" s="192"/>
+      <c r="E2" s="215">
         <v>2018</v>
       </c>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="197">
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="192"/>
+      <c r="I2" s="191">
         <v>2019</v>
       </c>
-      <c r="J2" s="199"/>
-      <c r="K2" s="199"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="200">
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="192"/>
+      <c r="M2" s="215">
         <v>2020</v>
       </c>
-      <c r="N2" s="199"/>
-      <c r="O2" s="199"/>
-      <c r="P2" s="226"/>
-      <c r="Q2" s="197" t="s">
+      <c r="N2" s="193"/>
+      <c r="O2" s="193"/>
+      <c r="P2" s="216"/>
+      <c r="Q2" s="191" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="199"/>
-      <c r="S2" s="198"/>
-      <c r="T2" s="219" t="s">
+      <c r="R2" s="193"/>
+      <c r="S2" s="192"/>
+      <c r="T2" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="217"/>
-      <c r="V2" s="217" t="s">
+      <c r="U2" s="206"/>
+      <c r="V2" s="206" t="s">
         <v>17</v>
       </c>
-      <c r="W2" s="217"/>
+      <c r="W2" s="206"/>
       <c r="X2" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="Y2" s="209" t="s">
+      <c r="Y2" s="201" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="206"/>
-      <c r="AA2" s="205" t="s">
+      <c r="Z2" s="198"/>
+      <c r="AA2" s="197" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="206"/>
+      <c r="AB2" s="198"/>
       <c r="AC2" s="158" t="s">
         <v>25</v>
       </c>
       <c r="AD2" s="161"/>
     </row>
-    <row r="3" spans="1:31" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="212"/>
+    <row r="3" spans="1:31" s="1" customFormat="1" ht="51.75" customHeight="1">
+      <c r="A3" s="221"/>
       <c r="B3" s="155"/>
       <c r="C3" s="155"/>
       <c r="D3" s="156"/>
-      <c r="E3" s="221" t="s">
+      <c r="E3" s="210" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222" t="s">
+      <c r="F3" s="211"/>
+      <c r="G3" s="211" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="223"/>
-      <c r="I3" s="220" t="s">
+      <c r="H3" s="212"/>
+      <c r="I3" s="209" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="221"/>
-      <c r="K3" s="222" t="s">
+      <c r="J3" s="210"/>
+      <c r="K3" s="211" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="223"/>
-      <c r="M3" s="221" t="s">
+      <c r="L3" s="212"/>
+      <c r="M3" s="210" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="222"/>
-      <c r="O3" s="222" t="s">
+      <c r="N3" s="211"/>
+      <c r="O3" s="211" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="224"/>
-      <c r="Q3" s="225" t="s">
+      <c r="P3" s="213"/>
+      <c r="Q3" s="214" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="222"/>
-      <c r="S3" s="223"/>
-      <c r="T3" s="210"/>
-      <c r="U3" s="218"/>
-      <c r="V3" s="218"/>
-      <c r="W3" s="218"/>
+      <c r="R3" s="211"/>
+      <c r="S3" s="212"/>
+      <c r="T3" s="202"/>
+      <c r="U3" s="207"/>
+      <c r="V3" s="207"/>
+      <c r="W3" s="207"/>
       <c r="X3" s="157"/>
-      <c r="Y3" s="210"/>
-      <c r="Z3" s="208"/>
-      <c r="AA3" s="207"/>
-      <c r="AB3" s="208"/>
+      <c r="Y3" s="202"/>
+      <c r="Z3" s="200"/>
+      <c r="AA3" s="199"/>
+      <c r="AB3" s="200"/>
       <c r="AC3" s="159"/>
       <c r="AD3" s="161"/>
       <c r="AE3" s="119"/>
     </row>
-    <row r="4" spans="1:31" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="213"/>
+    <row r="4" spans="1:31" s="1" customFormat="1" ht="64.5" customHeight="1">
+      <c r="A4" s="222"/>
       <c r="B4" s="154" t="s">
         <v>13</v>
       </c>
@@ -6194,7 +6152,7 @@
       </c>
       <c r="AE4" s="162"/>
     </row>
-    <row r="5" spans="1:31" s="15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" s="15" customFormat="1" ht="13.5" customHeight="1">
       <c r="A5" s="84" t="s">
         <v>0</v>
       </c>
@@ -6298,7 +6256,7 @@
       </c>
       <c r="AE5" s="53"/>
     </row>
-    <row r="6" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" s="15" customFormat="1" ht="13.8">
       <c r="A6" s="84" t="s">
         <v>1</v>
       </c>
@@ -6402,7 +6360,7 @@
       </c>
       <c r="AE6" s="53"/>
     </row>
-    <row r="7" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" s="15" customFormat="1" ht="13.8">
       <c r="A7" s="84" t="s">
         <v>2</v>
       </c>
@@ -6506,7 +6464,7 @@
       </c>
       <c r="AE7" s="53"/>
     </row>
-    <row r="8" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" s="15" customFormat="1" ht="13.8">
       <c r="A8" s="84" t="s">
         <v>3</v>
       </c>
@@ -6610,7 +6568,7 @@
       </c>
       <c r="AE8" s="53"/>
     </row>
-    <row r="9" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" s="15" customFormat="1" ht="13.8">
       <c r="A9" s="84" t="s">
         <v>4</v>
       </c>
@@ -6714,7 +6672,7 @@
       </c>
       <c r="AE9" s="53"/>
     </row>
-    <row r="10" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" s="15" customFormat="1" ht="13.8">
       <c r="A10" s="84" t="s">
         <v>5</v>
       </c>
@@ -6818,7 +6776,7 @@
       </c>
       <c r="AE10" s="53"/>
     </row>
-    <row r="11" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" s="15" customFormat="1" ht="13.8">
       <c r="A11" s="84" t="s">
         <v>6</v>
       </c>
@@ -6922,7 +6880,7 @@
       </c>
       <c r="AE11" s="53"/>
     </row>
-    <row r="12" spans="1:31" s="121" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" s="121" customFormat="1" ht="13.8">
       <c r="A12" s="122" t="s">
         <v>7</v>
       </c>
@@ -7026,7 +6984,7 @@
       </c>
       <c r="AE12" s="120"/>
     </row>
-    <row r="13" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" s="15" customFormat="1" ht="13.8">
       <c r="A13" s="84" t="s">
         <v>8</v>
       </c>
@@ -7130,7 +7088,7 @@
       </c>
       <c r="AE13" s="53"/>
     </row>
-    <row r="14" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" s="15" customFormat="1" ht="13.8">
       <c r="A14" s="84" t="s">
         <v>9</v>
       </c>
@@ -7234,7 +7192,7 @@
       </c>
       <c r="AE14" s="53"/>
     </row>
-    <row r="15" spans="1:31" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" s="15" customFormat="1" ht="13.8">
       <c r="A15" s="84" t="s">
         <v>10</v>
       </c>
@@ -7338,7 +7296,7 @@
       </c>
       <c r="AE15" s="53"/>
     </row>
-    <row r="16" spans="1:31" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" s="15" customFormat="1" thickBot="1">
       <c r="A16" s="85" t="s">
         <v>11</v>
       </c>
@@ -7442,7 +7400,7 @@
       </c>
       <c r="AE16" s="53"/>
     </row>
-    <row r="17" spans="1:31" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" s="15" customFormat="1" thickBot="1">
       <c r="A17" s="83"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -7474,7 +7432,7 @@
       <c r="AC17" s="17"/>
       <c r="AD17" s="17"/>
     </row>
-    <row r="18" spans="1:31" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" s="15" customFormat="1" thickBot="1">
       <c r="A18" s="91" t="s">
         <v>12</v>
       </c>
@@ -7588,11 +7546,14 @@
       <c r="AE18" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="19">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="I2:L2"/>
     <mergeCell ref="Y1:AC1"/>
     <mergeCell ref="AA2:AB3"/>
     <mergeCell ref="Y2:Z3"/>
-    <mergeCell ref="A2:A4"/>
     <mergeCell ref="T1:X1"/>
     <mergeCell ref="V2:W3"/>
     <mergeCell ref="T2:U3"/>
@@ -7605,10 +7566,6 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="I2:L2"/>
   </mergeCells>
   <conditionalFormatting sqref="T5:T16">
     <cfRule type="colorScale" priority="5">
@@ -7730,14 +7687,14 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.88671875" style="39" customWidth="1"/>
     <col min="2" max="3" width="14.109375" style="39" customWidth="1"/>
     <col min="4" max="5" width="12.88671875" style="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1">
       <c r="A1" s="36" t="s">
         <v>39</v>
       </c>
@@ -7752,7 +7709,7 @@
       </c>
       <c r="E1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
@@ -7770,7 +7727,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="34" t="s">
         <v>1</v>
       </c>
@@ -7788,7 +7745,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="34" t="s">
         <v>2</v>
       </c>
@@ -7806,7 +7763,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="34" t="s">
         <v>3</v>
       </c>
@@ -7824,7 +7781,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
@@ -7842,7 +7799,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="34" t="s">
         <v>5</v>
       </c>
@@ -7860,7 +7817,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="34" t="s">
         <v>6</v>
       </c>
@@ -7878,7 +7835,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="34" t="s">
         <v>7</v>
       </c>
@@ -7896,7 +7853,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="34" t="s">
         <v>8</v>
       </c>
@@ -7914,7 +7871,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="34" t="s">
         <v>9</v>
       </c>
@@ -7932,7 +7889,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="34" t="s">
         <v>10</v>
       </c>
@@ -7950,7 +7907,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="34" t="s">
         <v>11</v>
       </c>
@@ -7968,13 +7925,13 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="39" t="s">
         <v>41</v>
       </c>
@@ -7992,7 +7949,7 @@
       </c>
       <c r="E15" s="40"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" s="39" t="s">
         <v>42</v>
       </c>
@@ -8011,7 +7968,7 @@
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" s="39" t="s">
         <v>40</v>
       </c>
@@ -8030,7 +7987,7 @@
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" s="39" t="s">
         <v>43</v>
       </c>
@@ -8049,7 +8006,7 @@
       <c r="E19" s="40"/>
       <c r="F19" s="40"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20" s="39" t="s">
         <v>44</v>
       </c>
@@ -8068,7 +8025,7 @@
       <c r="E20" s="40"/>
       <c r="F20" s="40"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="39" t="s">
         <v>45</v>
       </c>
@@ -8087,7 +8044,7 @@
       <c r="E21" s="41"/>
       <c r="F21" s="41"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="B22" s="41">
         <f>B9/B20</f>
         <v>0.71963874624976298</v>
@@ -8134,13 +8091,13 @@
       <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="30" customHeight="1"/>
+    <row r="3" spans="2:7">
       <c r="C3" t="s">
         <v>46</v>
       </c>
@@ -8152,7 +8109,7 @@
       </c>
       <c r="F3" s="42"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7">
       <c r="B4" t="s">
         <v>52</v>
       </c>
@@ -8170,7 +8127,7 @@
       </c>
       <c r="F4" s="42"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7">
       <c r="B5" t="s">
         <v>53</v>
       </c>
@@ -8188,7 +8145,7 @@
       </c>
       <c r="F5" s="42"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7">
       <c r="B6" s="43" t="s">
         <v>47</v>
       </c>
@@ -8205,12 +8162,12 @@
         <v>5.5856054504256294</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7">
       <c r="B9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7">
       <c r="C10" t="s">
         <v>44</v>
       </c>
@@ -8224,7 +8181,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7">
       <c r="B11" t="s">
         <v>52</v>
       </c>
@@ -8246,7 +8203,7 @@
       </c>
       <c r="G11" s="44"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7">
       <c r="B12" t="s">
         <v>53</v>
       </c>
@@ -8268,7 +8225,7 @@
       </c>
       <c r="G12" s="44"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7">
       <c r="B13" s="43" t="s">
         <v>47</v>
       </c>
@@ -8290,16 +8247,16 @@
       </c>
       <c r="G13" s="44"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7">
       <c r="C14" s="42"/>
       <c r="D14" s="42"/>
       <c r="E14" s="42"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7">
       <c r="D15" s="42"/>
       <c r="E15" s="42"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7">
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
@@ -8307,11 +8264,11 @@
       <c r="F16" s="44"/>
       <c r="G16" s="44"/>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:5">
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:5">
       <c r="D18" s="45"/>
       <c r="E18" s="42"/>
     </row>
@@ -8329,25 +8286,25 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="35"/>
       <c r="B1" s="50" t="s">
         <v>51</v>
       </c>
       <c r="C1" s="35"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="B2" s="49" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="34" t="s">
         <v>0</v>
       </c>
@@ -8358,7 +8315,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="34" t="s">
         <v>1</v>
       </c>
@@ -8369,7 +8326,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="34" t="s">
         <v>2</v>
       </c>
@@ -8380,7 +8337,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="34" t="s">
         <v>3</v>
       </c>
@@ -8391,7 +8348,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="34" t="s">
         <v>4</v>
       </c>
@@ -8402,7 +8359,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="34" t="s">
         <v>5</v>
       </c>
@@ -8413,7 +8370,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="34" t="s">
         <v>6</v>
       </c>
@@ -8424,7 +8381,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="34" t="s">
         <v>7</v>
       </c>
@@ -8435,7 +8392,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="34" t="s">
         <v>8</v>
       </c>
@@ -8446,7 +8403,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="34" t="s">
         <v>9</v>
       </c>
@@ -8457,7 +8414,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="34" t="s">
         <v>10</v>
       </c>
@@ -8468,7 +8425,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="34" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
changed color in the redlight columns
</commit_message>
<xml_diff>
--- a/hon_planning_and_dev.xlsx
+++ b/hon_planning_and_dev.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\desktop\projects\pivot-yarok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA69EED3-11AD-45DF-B945-EAB9433BDB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D36CC3C-15E3-4E9C-ADAE-83803A87339F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="692" xr2:uid="{EE1E2518-0FD5-4401-B20A-1CAED4EDEA71}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="692" xr2:uid="{EE1E2518-0FD5-4401-B20A-1CAED4EDEA71}"/>
   </bookViews>
   <sheets>
     <sheet name="מדד על תכנון" sheetId="6" r:id="rId1"/>
@@ -1718,6 +1718,24 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1748,6 +1766,9 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1816,27 +1837,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4662,7 +4662,7 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4678,30 +4678,30 @@
   <sheetData>
     <row r="1" spans="1:22" ht="69.599999999999994" customHeight="1" thickBot="1">
       <c r="A1" s="166"/>
-      <c r="B1" s="184" t="s">
+      <c r="B1" s="190" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="185"/>
-      <c r="I1" s="185"/>
-      <c r="J1" s="185"/>
-      <c r="K1" s="186"/>
-      <c r="L1" s="187" t="s">
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="192"/>
+      <c r="L1" s="193" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="188"/>
-      <c r="N1" s="188"/>
-      <c r="O1" s="189"/>
-      <c r="P1" s="187" t="s">
+      <c r="M1" s="194"/>
+      <c r="N1" s="194"/>
+      <c r="O1" s="195"/>
+      <c r="P1" s="193" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="190"/>
-      <c r="R1" s="190"/>
-      <c r="S1" s="189"/>
+      <c r="Q1" s="196"/>
+      <c r="R1" s="196"/>
+      <c r="S1" s="195"/>
       <c r="T1" s="160" t="s">
         <v>65</v>
       </c>
@@ -4711,19 +4711,19 @@
       <c r="A2" s="183" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="191" t="s">
+      <c r="B2" s="197" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="192"/>
-      <c r="D2" s="191" t="s">
+      <c r="C2" s="198"/>
+      <c r="D2" s="197" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="192"/>
-      <c r="F2" s="191" t="s">
+      <c r="E2" s="198"/>
+      <c r="F2" s="197" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="193"/>
-      <c r="H2" s="192"/>
+      <c r="G2" s="199"/>
+      <c r="H2" s="198"/>
       <c r="I2" s="163">
         <v>2018</v>
       </c>
@@ -4733,25 +4733,25 @@
       <c r="K2" s="165">
         <v>2020</v>
       </c>
-      <c r="L2" s="219" t="s">
+      <c r="L2" s="185" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="218" t="s">
+      <c r="M2" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="218" t="s">
+      <c r="N2" s="184" t="s">
         <v>37</v>
       </c>
       <c r="O2" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="219" t="s">
+      <c r="P2" s="185" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="218" t="s">
+      <c r="Q2" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="218" t="s">
+      <c r="R2" s="184" t="s">
         <v>34</v>
       </c>
       <c r="S2" s="158" t="s">
@@ -4761,7 +4761,7 @@
       <c r="V2" s="15"/>
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" ht="62.25" customHeight="1">
-      <c r="A3" s="223"/>
+      <c r="A3" s="189"/>
       <c r="B3" s="5" t="s">
         <v>32</v>
       </c>
@@ -4792,25 +4792,25 @@
       <c r="K3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="219" t="s">
+      <c r="L3" s="185" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="218" t="s">
+      <c r="M3" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="218" t="s">
+      <c r="N3" s="184" t="s">
         <v>37</v>
       </c>
       <c r="O3" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="219" t="s">
+      <c r="P3" s="185" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="218" t="s">
+      <c r="Q3" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="218" t="s">
+      <c r="R3" s="184" t="s">
         <v>34</v>
       </c>
       <c r="S3" s="158" t="s">
@@ -5903,7 +5903,7 @@
   <dimension ref="A1:AE18"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5920,149 +5920,149 @@
   <sheetData>
     <row r="1" spans="1:31" ht="22.95" customHeight="1" thickBot="1">
       <c r="A1" s="103"/>
-      <c r="B1" s="217" t="s">
+      <c r="B1" s="200" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="185"/>
-      <c r="I1" s="185"/>
-      <c r="J1" s="185"/>
-      <c r="K1" s="185"/>
-      <c r="L1" s="185"/>
-      <c r="M1" s="185"/>
-      <c r="N1" s="185"/>
-      <c r="O1" s="185"/>
-      <c r="P1" s="185"/>
-      <c r="Q1" s="185"/>
-      <c r="R1" s="185"/>
-      <c r="S1" s="186"/>
-      <c r="T1" s="203" t="s">
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="191"/>
+      <c r="M1" s="191"/>
+      <c r="N1" s="191"/>
+      <c r="O1" s="191"/>
+      <c r="P1" s="191"/>
+      <c r="Q1" s="191"/>
+      <c r="R1" s="191"/>
+      <c r="S1" s="192"/>
+      <c r="T1" s="210" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="204"/>
-      <c r="V1" s="204"/>
-      <c r="W1" s="204"/>
-      <c r="X1" s="205"/>
-      <c r="Y1" s="194" t="s">
+      <c r="U1" s="211"/>
+      <c r="V1" s="211"/>
+      <c r="W1" s="211"/>
+      <c r="X1" s="212"/>
+      <c r="Y1" s="201" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="195"/>
-      <c r="AA1" s="195"/>
-      <c r="AB1" s="195"/>
-      <c r="AC1" s="196"/>
+      <c r="Z1" s="202"/>
+      <c r="AA1" s="202"/>
+      <c r="AB1" s="202"/>
+      <c r="AC1" s="203"/>
       <c r="AD1" s="160" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="17.7" customHeight="1">
-      <c r="A2" s="220" t="s">
+      <c r="A2" s="186" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="191" t="s">
+      <c r="B2" s="197" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="193"/>
-      <c r="D2" s="192"/>
-      <c r="E2" s="215">
+      <c r="C2" s="199"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="222">
         <v>2018</v>
       </c>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="192"/>
-      <c r="I2" s="191">
+      <c r="F2" s="199"/>
+      <c r="G2" s="199"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="197">
         <v>2019</v>
       </c>
-      <c r="J2" s="193"/>
-      <c r="K2" s="193"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="215">
+      <c r="J2" s="199"/>
+      <c r="K2" s="199"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="222">
         <v>2020</v>
       </c>
-      <c r="N2" s="193"/>
-      <c r="O2" s="193"/>
-      <c r="P2" s="216"/>
-      <c r="Q2" s="191" t="s">
+      <c r="N2" s="199"/>
+      <c r="O2" s="199"/>
+      <c r="P2" s="223"/>
+      <c r="Q2" s="197" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="193"/>
-      <c r="S2" s="192"/>
-      <c r="T2" s="208" t="s">
+      <c r="R2" s="199"/>
+      <c r="S2" s="198"/>
+      <c r="T2" s="215" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="206"/>
-      <c r="V2" s="206" t="s">
+      <c r="U2" s="213"/>
+      <c r="V2" s="213" t="s">
         <v>17</v>
       </c>
-      <c r="W2" s="206"/>
+      <c r="W2" s="213"/>
       <c r="X2" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="Y2" s="201" t="s">
+      <c r="Y2" s="208" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="198"/>
-      <c r="AA2" s="197" t="s">
+      <c r="Z2" s="205"/>
+      <c r="AA2" s="204" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="198"/>
+      <c r="AB2" s="205"/>
       <c r="AC2" s="158" t="s">
         <v>25</v>
       </c>
       <c r="AD2" s="161"/>
     </row>
     <row r="3" spans="1:31" s="1" customFormat="1" ht="51.75" customHeight="1">
-      <c r="A3" s="221"/>
+      <c r="A3" s="187"/>
       <c r="B3" s="155"/>
       <c r="C3" s="155"/>
       <c r="D3" s="156"/>
-      <c r="E3" s="210" t="s">
+      <c r="E3" s="217" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="211"/>
-      <c r="G3" s="211" t="s">
+      <c r="F3" s="218"/>
+      <c r="G3" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="212"/>
-      <c r="I3" s="209" t="s">
+      <c r="H3" s="219"/>
+      <c r="I3" s="216" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="210"/>
-      <c r="K3" s="211" t="s">
+      <c r="J3" s="217"/>
+      <c r="K3" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="212"/>
-      <c r="M3" s="210" t="s">
+      <c r="L3" s="219"/>
+      <c r="M3" s="217" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="211"/>
-      <c r="O3" s="211" t="s">
+      <c r="N3" s="218"/>
+      <c r="O3" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="213"/>
-      <c r="Q3" s="214" t="s">
+      <c r="P3" s="220"/>
+      <c r="Q3" s="221" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="211"/>
-      <c r="S3" s="212"/>
-      <c r="T3" s="202"/>
-      <c r="U3" s="207"/>
-      <c r="V3" s="207"/>
-      <c r="W3" s="207"/>
+      <c r="R3" s="218"/>
+      <c r="S3" s="219"/>
+      <c r="T3" s="209"/>
+      <c r="U3" s="214"/>
+      <c r="V3" s="214"/>
+      <c r="W3" s="214"/>
       <c r="X3" s="157"/>
-      <c r="Y3" s="202"/>
-      <c r="Z3" s="200"/>
-      <c r="AA3" s="199"/>
-      <c r="AB3" s="200"/>
+      <c r="Y3" s="209"/>
+      <c r="Z3" s="207"/>
+      <c r="AA3" s="206"/>
+      <c r="AB3" s="207"/>
       <c r="AC3" s="159"/>
       <c r="AD3" s="161"/>
       <c r="AE3" s="119"/>
     </row>
     <row r="4" spans="1:31" s="1" customFormat="1" ht="64.5" customHeight="1">
-      <c r="A4" s="222"/>
+      <c r="A4" s="188"/>
       <c r="B4" s="154" t="s">
         <v>13</v>
       </c>
@@ -7547,6 +7547,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="E2:H2"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B1:S1"/>
     <mergeCell ref="Q2:S2"/>
@@ -7563,9 +7566,6 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="T5:T16">
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
changed color of titles
</commit_message>
<xml_diff>
--- a/hon_planning_and_dev.xlsx
+++ b/hon_planning_and_dev.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adavi\desktop\projects\pivot-yarok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D36CC3C-15E3-4E9C-ADAE-83803A87339F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D1F554-3848-44C1-B653-280980E7EE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="692" xr2:uid="{EE1E2518-0FD5-4401-B20A-1CAED4EDEA71}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="692" xr2:uid="{EE1E2518-0FD5-4401-B20A-1CAED4EDEA71}"/>
   </bookViews>
   <sheets>
     <sheet name="מדד על תכנון" sheetId="6" r:id="rId1"/>
@@ -1766,6 +1766,18 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1820,22 +1832,10 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -4661,8 +4661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814DFBB6-7E08-4D07-BC22-E38BA1AEF93F}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5809,17 +5809,17 @@
     <mergeCell ref="F2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:I15">
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
       <formula>$I$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J15">
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>$J$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:N15">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>$K$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5834,7 +5834,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>$L$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5849,7 +5849,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>$M$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5864,7 +5864,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>$N$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5879,17 +5879,17 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>$O$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:T15">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:T15">
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>$T$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5903,7 +5903,7 @@
   <dimension ref="A1:AE18"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5920,7 +5920,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="22.95" customHeight="1" thickBot="1">
       <c r="A1" s="103"/>
-      <c r="B1" s="200" t="s">
+      <c r="B1" s="204" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="191"/>
@@ -5940,20 +5940,20 @@
       <c r="Q1" s="191"/>
       <c r="R1" s="191"/>
       <c r="S1" s="192"/>
-      <c r="T1" s="210" t="s">
+      <c r="T1" s="214" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="211"/>
-      <c r="V1" s="211"/>
-      <c r="W1" s="211"/>
-      <c r="X1" s="212"/>
-      <c r="Y1" s="201" t="s">
+      <c r="U1" s="215"/>
+      <c r="V1" s="215"/>
+      <c r="W1" s="215"/>
+      <c r="X1" s="216"/>
+      <c r="Y1" s="205" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="202"/>
-      <c r="AA1" s="202"/>
-      <c r="AB1" s="202"/>
-      <c r="AC1" s="203"/>
+      <c r="Z1" s="206"/>
+      <c r="AA1" s="206"/>
+      <c r="AB1" s="206"/>
+      <c r="AC1" s="207"/>
       <c r="AD1" s="160" t="s">
         <v>66</v>
       </c>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="C2" s="199"/>
       <c r="D2" s="198"/>
-      <c r="E2" s="222">
+      <c r="E2" s="202">
         <v>2018</v>
       </c>
       <c r="F2" s="199"/>
@@ -5979,36 +5979,36 @@
       <c r="J2" s="199"/>
       <c r="K2" s="199"/>
       <c r="L2" s="198"/>
-      <c r="M2" s="222">
+      <c r="M2" s="202">
         <v>2020</v>
       </c>
       <c r="N2" s="199"/>
       <c r="O2" s="199"/>
-      <c r="P2" s="223"/>
+      <c r="P2" s="203"/>
       <c r="Q2" s="197" t="s">
         <v>38</v>
       </c>
       <c r="R2" s="199"/>
       <c r="S2" s="198"/>
-      <c r="T2" s="215" t="s">
+      <c r="T2" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="213"/>
-      <c r="V2" s="213" t="s">
+      <c r="U2" s="217"/>
+      <c r="V2" s="217" t="s">
         <v>17</v>
       </c>
-      <c r="W2" s="213"/>
+      <c r="W2" s="217"/>
       <c r="X2" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="Y2" s="208" t="s">
+      <c r="Y2" s="212" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="205"/>
-      <c r="AA2" s="204" t="s">
+      <c r="Z2" s="209"/>
+      <c r="AA2" s="208" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="205"/>
+      <c r="AB2" s="209"/>
       <c r="AC2" s="158" t="s">
         <v>25</v>
       </c>
@@ -6019,44 +6019,44 @@
       <c r="B3" s="155"/>
       <c r="C3" s="155"/>
       <c r="D3" s="156"/>
-      <c r="E3" s="217" t="s">
+      <c r="E3" s="221" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="218"/>
-      <c r="G3" s="218" t="s">
+      <c r="F3" s="200"/>
+      <c r="G3" s="200" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="219"/>
-      <c r="I3" s="216" t="s">
+      <c r="H3" s="201"/>
+      <c r="I3" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="217"/>
-      <c r="K3" s="218" t="s">
+      <c r="J3" s="221"/>
+      <c r="K3" s="200" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="219"/>
-      <c r="M3" s="217" t="s">
+      <c r="L3" s="201"/>
+      <c r="M3" s="221" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="218"/>
-      <c r="O3" s="218" t="s">
+      <c r="N3" s="200"/>
+      <c r="O3" s="200" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="220"/>
-      <c r="Q3" s="221" t="s">
+      <c r="P3" s="222"/>
+      <c r="Q3" s="223" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="218"/>
-      <c r="S3" s="219"/>
-      <c r="T3" s="209"/>
-      <c r="U3" s="214"/>
-      <c r="V3" s="214"/>
-      <c r="W3" s="214"/>
+      <c r="R3" s="200"/>
+      <c r="S3" s="201"/>
+      <c r="T3" s="213"/>
+      <c r="U3" s="218"/>
+      <c r="V3" s="218"/>
+      <c r="W3" s="218"/>
       <c r="X3" s="157"/>
-      <c r="Y3" s="209"/>
-      <c r="Z3" s="207"/>
-      <c r="AA3" s="206"/>
-      <c r="AB3" s="207"/>
+      <c r="Y3" s="213"/>
+      <c r="Z3" s="211"/>
+      <c r="AA3" s="210"/>
+      <c r="AB3" s="211"/>
       <c r="AC3" s="159"/>
       <c r="AD3" s="161"/>
       <c r="AE3" s="119"/>
@@ -7547,6 +7547,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="Y1:AC1"/>
+    <mergeCell ref="AA2:AB3"/>
+    <mergeCell ref="Y2:Z3"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="V2:W3"/>
+    <mergeCell ref="T2:U3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="E2:H2"/>
@@ -7554,12 +7560,6 @@
     <mergeCell ref="B1:S1"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="I2:L2"/>
-    <mergeCell ref="Y1:AC1"/>
-    <mergeCell ref="AA2:AB3"/>
-    <mergeCell ref="Y2:Z3"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="V2:W3"/>
-    <mergeCell ref="T2:U3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
@@ -7578,7 +7578,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
       <formula>$T$18</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7593,7 +7593,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
       <formula>$U$18</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7608,7 +7608,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
       <formula>$V$18</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7625,7 +7625,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W5:X16">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>$W$18</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7640,37 +7640,37 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>$X$18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y5:Y16">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y5:AD16">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:Z16">
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>$Z$18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA5:AA16">
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>$AA$18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5:AB16">
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>$AB$18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD5:AD16">
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>$AD$18</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8062,20 +8062,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="cellIs" dxfId="3" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="135" operator="equal">
       <formula>$B$15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="cellIs" dxfId="2" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="133" operator="equal">
       <formula>$C$15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>$D$15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="137" operator="equal">
       <formula>$E$15</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>